<commit_message>
Nouvelle feuille du pic avec la nouvelle repartition des pattes
</commit_message>
<xml_diff>
--- a/PIC Pinout.xlsx
+++ b/PIC Pinout.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocal\Desktop\Elec_synthe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20475" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="182">
   <si>
     <t>PIC32MX575F512H-80I/PT  Pinout</t>
   </si>
@@ -556,6 +561,15 @@
   </si>
   <si>
     <t>Quartz</t>
+  </si>
+  <si>
+    <t>2OC</t>
+  </si>
+  <si>
+    <t>2SPI</t>
+  </si>
+  <si>
+    <t>OC</t>
   </si>
 </sst>
 </file>
@@ -630,7 +644,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,6 +783,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -1217,7 +1237,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1294,6 +1314,18 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,18 +1344,9 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="371">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1700,6 +1723,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2025,38 +2056,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:XEJ72"/>
+  <dimension ref="B1:XEJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BG8" sqref="BG8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BS16" sqref="BS16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="1.1640625" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.83203125" customWidth="1"/>
-    <col min="6" max="6" width="1.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="1.125" customWidth="1"/>
+    <col min="3" max="3" width="5.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.875" customWidth="1"/>
+    <col min="6" max="6" width="1.125" customWidth="1"/>
     <col min="7" max="42" width="3.5" customWidth="1"/>
-    <col min="43" max="43" width="1.1640625" customWidth="1"/>
-    <col min="44" max="52" width="3.6640625" customWidth="1"/>
-    <col min="53" max="57" width="3.5" customWidth="1"/>
-    <col min="58" max="58" width="1.1640625" customWidth="1"/>
+    <col min="43" max="43" width="1.125" customWidth="1"/>
+    <col min="44" max="45" width="3.5" customWidth="1"/>
+    <col min="46" max="54" width="3.625" customWidth="1"/>
+    <col min="55" max="57" width="3.5" customWidth="1"/>
+    <col min="58" max="58" width="1.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:58" ht="21">
-      <c r="D2" s="65" t="s">
+    <row r="1" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="AU1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="2:58" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="D2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-    </row>
-    <row r="3" spans="2:58" s="28" customFormat="1" ht="120" customHeight="1">
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="AR2">
+        <v>3</v>
+      </c>
+      <c r="AS2">
+        <v>2</v>
+      </c>
+      <c r="AT2">
+        <v>1</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW2">
+        <v>9</v>
+      </c>
+      <c r="AX2">
+        <v>5</v>
+      </c>
+      <c r="AY2">
+        <v>8</v>
+      </c>
+      <c r="AZ2">
+        <v>6</v>
+      </c>
+      <c r="BA2">
+        <v>2</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="2:58" s="28" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="29"/>
       <c r="G3" s="28" t="s">
         <v>124</v>
@@ -2164,49 +2237,49 @@
         <v>158</v>
       </c>
       <c r="AR3" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS3" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="AT3" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="AS3" s="28" t="s">
+      <c r="AU3" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="AT3" s="28" t="s">
+      <c r="AV3" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="AU3" s="28" t="s">
+      <c r="AW3" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="AV3" s="28" t="s">
+      <c r="AX3" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="AW3" s="28" t="s">
+      <c r="AY3" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="AX3" s="28" t="s">
+      <c r="AZ3" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="AY3" s="28" t="s">
+      <c r="BA3" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="AZ3" s="28" t="s">
+      <c r="BB3" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="BA3" s="28" t="s">
+      <c r="BC3" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="BB3" s="28" t="s">
+      <c r="BD3" s="28" t="s">
         <v>175</v>
-      </c>
-      <c r="BC3" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="BD3" s="28" t="s">
-        <v>178</v>
       </c>
       <c r="BE3" s="28" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="2:58" ht="8" customHeight="1">
+    <row r="4" spans="2:58" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
@@ -2265,7 +2338,7 @@
       <c r="BE4" s="14"/>
       <c r="BF4" s="14"/>
     </row>
-    <row r="5" spans="2:58">
+    <row r="5" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B5" s="48"/>
       <c r="C5" s="3" t="s">
         <v>60</v>
@@ -2315,14 +2388,14 @@
       <c r="AP5" s="6"/>
       <c r="AQ5" s="48"/>
       <c r="AR5" s="6"/>
-      <c r="AS5" s="30"/>
-      <c r="AT5" s="6"/>
-      <c r="AU5" s="6"/>
-      <c r="AV5" s="6"/>
-      <c r="AW5" s="6"/>
-      <c r="AX5" s="6"/>
-      <c r="AY5" s="6"/>
-      <c r="AZ5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="66"/>
+      <c r="AU5" s="66"/>
+      <c r="AV5" s="66"/>
+      <c r="AW5" s="66"/>
+      <c r="AX5" s="53"/>
+      <c r="AY5" s="66"/>
+      <c r="AZ5" s="66"/>
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
       <c r="BC5" s="6"/>
@@ -2330,7 +2403,7 @@
       <c r="BE5" s="6"/>
       <c r="BF5" s="48"/>
     </row>
-    <row r="6" spans="2:58">
+    <row r="6" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B6" s="48"/>
       <c r="C6" s="3" t="s">
         <v>61</v>
@@ -2380,14 +2453,14 @@
       <c r="AP6" s="6"/>
       <c r="AQ6" s="48"/>
       <c r="AR6" s="6"/>
-      <c r="AS6" s="30"/>
-      <c r="AT6" s="6"/>
-      <c r="AU6" s="6"/>
-      <c r="AV6" s="6"/>
-      <c r="AW6" s="6"/>
-      <c r="AX6" s="6"/>
-      <c r="AY6" s="6"/>
-      <c r="AZ6" s="6"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="66"/>
+      <c r="AU6" s="66"/>
+      <c r="AV6" s="66"/>
+      <c r="AW6" s="53"/>
+      <c r="AX6" s="66"/>
+      <c r="AY6" s="66"/>
+      <c r="AZ6" s="66"/>
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
       <c r="BC6" s="6"/>
@@ -2395,7 +2468,7 @@
       <c r="BE6" s="6"/>
       <c r="BF6" s="48"/>
     </row>
-    <row r="7" spans="2:58">
+    <row r="7" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B7" s="48"/>
       <c r="C7" s="3" t="s">
         <v>62</v>
@@ -2445,14 +2518,14 @@
       <c r="AP7" s="6"/>
       <c r="AQ7" s="48"/>
       <c r="AR7" s="6"/>
-      <c r="AS7" s="30"/>
-      <c r="AT7" s="6"/>
-      <c r="AU7" s="6"/>
-      <c r="AV7" s="6"/>
-      <c r="AW7" s="6"/>
-      <c r="AX7" s="6"/>
-      <c r="AY7" s="6"/>
-      <c r="AZ7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="66"/>
+      <c r="AU7" s="66"/>
+      <c r="AV7" s="66"/>
+      <c r="AW7" s="53"/>
+      <c r="AX7" s="66"/>
+      <c r="AY7" s="66"/>
+      <c r="AZ7" s="66"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
       <c r="BC7" s="6"/>
@@ -2460,7 +2533,7 @@
       <c r="BE7" s="6"/>
       <c r="BF7" s="48"/>
     </row>
-    <row r="8" spans="2:58">
+    <row r="8" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B8" s="48"/>
       <c r="C8" s="3" t="s">
         <v>63</v>
@@ -2511,13 +2584,13 @@
       <c r="AQ8" s="48"/>
       <c r="AR8" s="6"/>
       <c r="AS8" s="6"/>
-      <c r="AT8" s="30"/>
-      <c r="AU8" s="6"/>
-      <c r="AV8" s="6"/>
-      <c r="AW8" s="6"/>
-      <c r="AX8" s="6"/>
-      <c r="AY8" s="6"/>
-      <c r="AZ8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="53"/>
+      <c r="AV8" s="66"/>
+      <c r="AW8" s="66"/>
+      <c r="AX8" s="66"/>
+      <c r="AY8" s="66"/>
+      <c r="AZ8" s="66"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
       <c r="BC8" s="6"/>
@@ -2525,7 +2598,7 @@
       <c r="BE8" s="6"/>
       <c r="BF8" s="48"/>
     </row>
-    <row r="9" spans="2:58">
+    <row r="9" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B9" s="48"/>
       <c r="C9" s="3" t="s">
         <v>64</v>
@@ -2576,13 +2649,13 @@
       <c r="AQ9" s="48"/>
       <c r="AR9" s="6"/>
       <c r="AS9" s="6"/>
-      <c r="AT9" s="30"/>
-      <c r="AU9" s="6"/>
-      <c r="AV9" s="6"/>
-      <c r="AW9" s="6"/>
-      <c r="AX9" s="6"/>
-      <c r="AY9" s="6"/>
-      <c r="AZ9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="66"/>
+      <c r="AV9" s="66"/>
+      <c r="AW9" s="53"/>
+      <c r="AX9" s="66"/>
+      <c r="AY9" s="66"/>
+      <c r="AZ9" s="66"/>
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
       <c r="BC9" s="6"/>
@@ -2590,7 +2663,7 @@
       <c r="BE9" s="6"/>
       <c r="BF9" s="48"/>
     </row>
-    <row r="10" spans="2:58">
+    <row r="10" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B10" s="48"/>
       <c r="C10" s="3" t="s">
         <v>65</v>
@@ -2641,13 +2714,13 @@
       <c r="AQ10" s="48"/>
       <c r="AR10" s="6"/>
       <c r="AS10" s="6"/>
-      <c r="AT10" s="30"/>
-      <c r="AU10" s="6"/>
-      <c r="AV10" s="6"/>
-      <c r="AW10" s="6"/>
-      <c r="AX10" s="6"/>
-      <c r="AY10" s="6"/>
-      <c r="AZ10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="53"/>
+      <c r="AV10" s="66"/>
+      <c r="AW10" s="66"/>
+      <c r="AX10" s="66"/>
+      <c r="AY10" s="66"/>
+      <c r="AZ10" s="66"/>
       <c r="BA10" s="6"/>
       <c r="BB10" s="6"/>
       <c r="BC10" s="6"/>
@@ -2655,7 +2728,7 @@
       <c r="BE10" s="6"/>
       <c r="BF10" s="48"/>
     </row>
-    <row r="11" spans="2:58">
+    <row r="11" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B11" s="48"/>
       <c r="C11" s="3" t="s">
         <v>66</v>
@@ -2667,46 +2740,46 @@
         <v>7</v>
       </c>
       <c r="F11" s="48"/>
-      <c r="G11" s="62" t="s">
+      <c r="G11" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
-      <c r="X11" s="63"/>
-      <c r="Y11" s="63"/>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="63"/>
-      <c r="AB11" s="63"/>
-      <c r="AC11" s="63"/>
-      <c r="AD11" s="63"/>
-      <c r="AE11" s="63"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="63"/>
-      <c r="AH11" s="63"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="63"/>
-      <c r="AL11" s="63"/>
-      <c r="AM11" s="63"/>
-      <c r="AN11" s="63"/>
-      <c r="AO11" s="63"/>
-      <c r="AP11" s="64"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="58"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="58"/>
+      <c r="AF11" s="58"/>
+      <c r="AG11" s="58"/>
+      <c r="AH11" s="58"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AK11" s="58"/>
+      <c r="AL11" s="58"/>
+      <c r="AM11" s="58"/>
+      <c r="AN11" s="58"/>
+      <c r="AO11" s="58"/>
+      <c r="AP11" s="59"/>
       <c r="AQ11" s="48"/>
-      <c r="AR11" s="49"/>
+      <c r="AR11" s="67"/>
       <c r="AS11" s="49"/>
       <c r="AT11" s="49"/>
       <c r="AU11" s="49"/>
@@ -2722,7 +2795,7 @@
       <c r="BE11" s="49"/>
       <c r="BF11" s="48"/>
     </row>
-    <row r="12" spans="2:58">
+    <row r="12" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B12" s="48"/>
       <c r="C12" s="3" t="s">
         <v>67</v>
@@ -2773,11 +2846,11 @@
       <c r="AQ12" s="48"/>
       <c r="AR12" s="6"/>
       <c r="AS12" s="6"/>
-      <c r="AT12" s="30"/>
-      <c r="AU12" s="6"/>
-      <c r="AV12" s="6"/>
-      <c r="AW12" s="6"/>
-      <c r="AX12" s="6"/>
+      <c r="AT12" s="66"/>
+      <c r="AU12" s="66"/>
+      <c r="AV12" s="66"/>
+      <c r="AW12" s="53"/>
+      <c r="AX12" s="66"/>
       <c r="AY12" s="6"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
@@ -2787,7 +2860,7 @@
       <c r="BE12" s="6"/>
       <c r="BF12" s="48"/>
     </row>
-    <row r="13" spans="2:58">
+    <row r="13" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B13" s="48"/>
       <c r="C13" s="3" t="s">
         <v>68</v>
@@ -2799,44 +2872,44 @@
         <v>9</v>
       </c>
       <c r="F13" s="48"/>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
-      <c r="AH13" s="60"/>
-      <c r="AI13" s="60"/>
-      <c r="AJ13" s="60"/>
-      <c r="AK13" s="60"/>
-      <c r="AL13" s="60"/>
-      <c r="AM13" s="60"/>
-      <c r="AN13" s="60"/>
-      <c r="AO13" s="60"/>
-      <c r="AP13" s="61"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="64"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="64"/>
+      <c r="T13" s="64"/>
+      <c r="U13" s="64"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="64"/>
+      <c r="X13" s="64"/>
+      <c r="Y13" s="64"/>
+      <c r="Z13" s="64"/>
+      <c r="AA13" s="64"/>
+      <c r="AB13" s="64"/>
+      <c r="AC13" s="64"/>
+      <c r="AD13" s="64"/>
+      <c r="AE13" s="64"/>
+      <c r="AF13" s="64"/>
+      <c r="AG13" s="64"/>
+      <c r="AH13" s="64"/>
+      <c r="AI13" s="64"/>
+      <c r="AJ13" s="64"/>
+      <c r="AK13" s="64"/>
+      <c r="AL13" s="64"/>
+      <c r="AM13" s="64"/>
+      <c r="AN13" s="64"/>
+      <c r="AO13" s="64"/>
+      <c r="AP13" s="65"/>
       <c r="AQ13" s="48"/>
       <c r="AR13" s="50"/>
       <c r="AS13" s="50"/>
@@ -2854,7 +2927,7 @@
       <c r="BE13" s="50"/>
       <c r="BF13" s="48"/>
     </row>
-    <row r="14" spans="2:58">
+    <row r="14" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B14" s="48"/>
       <c r="C14" s="3" t="s">
         <v>69</v>
@@ -2866,44 +2939,44 @@
         <v>10</v>
       </c>
       <c r="F14" s="48"/>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="57"/>
-      <c r="AA14" s="57"/>
-      <c r="AB14" s="57"/>
-      <c r="AC14" s="57"/>
-      <c r="AD14" s="57"/>
-      <c r="AE14" s="57"/>
-      <c r="AF14" s="57"/>
-      <c r="AG14" s="57"/>
-      <c r="AH14" s="57"/>
-      <c r="AI14" s="57"/>
-      <c r="AJ14" s="57"/>
-      <c r="AK14" s="57"/>
-      <c r="AL14" s="57"/>
-      <c r="AM14" s="57"/>
-      <c r="AN14" s="57"/>
-      <c r="AO14" s="57"/>
-      <c r="AP14" s="58"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="61"/>
+      <c r="U14" s="61"/>
+      <c r="V14" s="61"/>
+      <c r="W14" s="61"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="61"/>
+      <c r="Z14" s="61"/>
+      <c r="AA14" s="61"/>
+      <c r="AB14" s="61"/>
+      <c r="AC14" s="61"/>
+      <c r="AD14" s="61"/>
+      <c r="AE14" s="61"/>
+      <c r="AF14" s="61"/>
+      <c r="AG14" s="61"/>
+      <c r="AH14" s="61"/>
+      <c r="AI14" s="61"/>
+      <c r="AJ14" s="61"/>
+      <c r="AK14" s="61"/>
+      <c r="AL14" s="61"/>
+      <c r="AM14" s="61"/>
+      <c r="AN14" s="61"/>
+      <c r="AO14" s="61"/>
+      <c r="AP14" s="62"/>
       <c r="AQ14" s="48"/>
       <c r="AR14" s="51"/>
       <c r="AS14" s="51"/>
@@ -2921,7 +2994,7 @@
       <c r="BE14" s="51"/>
       <c r="BF14" s="48"/>
     </row>
-    <row r="15" spans="2:58">
+    <row r="15" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B15" s="48"/>
       <c r="C15" s="3" t="s">
         <v>70</v>
@@ -2975,9 +3048,9 @@
       <c r="AT15" s="6"/>
       <c r="AU15" s="6"/>
       <c r="AV15" s="6"/>
-      <c r="AW15" s="52"/>
-      <c r="AX15" s="6"/>
-      <c r="AY15" s="6"/>
+      <c r="AW15" s="66"/>
+      <c r="AX15" s="53"/>
+      <c r="AY15" s="66"/>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
       <c r="BB15" s="6"/>
@@ -2986,7 +3059,7 @@
       <c r="BE15" s="6"/>
       <c r="BF15" s="48"/>
     </row>
-    <row r="16" spans="2:58">
+    <row r="16" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B16" s="48"/>
       <c r="C16" s="3" t="s">
         <v>71</v>
@@ -3040,9 +3113,9 @@
       <c r="AT16" s="6"/>
       <c r="AU16" s="6"/>
       <c r="AV16" s="6"/>
-      <c r="AW16" s="52"/>
-      <c r="AX16" s="6"/>
-      <c r="AY16" s="6"/>
+      <c r="AW16" s="66"/>
+      <c r="AX16" s="66"/>
+      <c r="AY16" s="53"/>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="6"/>
@@ -3051,7 +3124,7 @@
       <c r="BE16" s="6"/>
       <c r="BF16" s="48"/>
     </row>
-    <row r="17" spans="2:58 16364:16364">
+    <row r="17" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B17" s="48"/>
       <c r="C17" s="3" t="s">
         <v>72</v>
@@ -3105,9 +3178,9 @@
       <c r="AT17" s="6"/>
       <c r="AU17" s="6"/>
       <c r="AV17" s="6"/>
-      <c r="AW17" s="52"/>
-      <c r="AX17" s="6"/>
-      <c r="AY17" s="6"/>
+      <c r="AW17" s="66"/>
+      <c r="AX17" s="66"/>
+      <c r="AY17" s="53"/>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
@@ -3116,7 +3189,7 @@
       <c r="BE17" s="6"/>
       <c r="BF17" s="48"/>
     </row>
-    <row r="18" spans="2:58 16364:16364">
+    <row r="18" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B18" s="48"/>
       <c r="C18" s="3" t="s">
         <v>73</v>
@@ -3166,22 +3239,22 @@
       <c r="AP18" s="6"/>
       <c r="AQ18" s="48"/>
       <c r="AR18" s="6"/>
-      <c r="AS18" s="6"/>
+      <c r="AS18" s="52"/>
       <c r="AT18" s="6"/>
       <c r="AU18" s="6"/>
       <c r="AV18" s="6"/>
-      <c r="AW18" s="52"/>
-      <c r="AX18" s="6"/>
-      <c r="AY18" s="6"/>
+      <c r="AW18" s="66"/>
+      <c r="AX18" s="66"/>
+      <c r="AY18" s="53"/>
       <c r="AZ18" s="6"/>
       <c r="BA18" s="6"/>
       <c r="BB18" s="6"/>
       <c r="BC18" s="6"/>
-      <c r="BD18" s="52"/>
+      <c r="BD18" s="6"/>
       <c r="BE18" s="6"/>
       <c r="BF18" s="48"/>
     </row>
-    <row r="19" spans="2:58 16364:16364">
+    <row r="19" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B19" s="48"/>
       <c r="C19" s="3" t="s">
         <v>74</v>
@@ -3230,23 +3303,23 @@
       <c r="AO19" s="38"/>
       <c r="AP19" s="6"/>
       <c r="AQ19" s="48"/>
-      <c r="AR19" s="6"/>
-      <c r="AS19" s="6"/>
+      <c r="AR19" s="53"/>
+      <c r="AS19" s="52"/>
       <c r="AT19" s="6"/>
       <c r="AU19" s="6"/>
-      <c r="AV19" s="52"/>
-      <c r="AW19" s="52"/>
-      <c r="AX19" s="52"/>
-      <c r="AY19" s="6"/>
-      <c r="AZ19" s="6"/>
+      <c r="AV19" s="6"/>
+      <c r="AW19" s="66"/>
+      <c r="AX19" s="66"/>
+      <c r="AY19" s="66"/>
+      <c r="AZ19" s="52"/>
       <c r="BA19" s="6"/>
       <c r="BB19" s="6"/>
-      <c r="BC19" s="53"/>
-      <c r="BD19" s="52"/>
+      <c r="BC19" s="6"/>
+      <c r="BD19" s="6"/>
       <c r="BE19" s="6"/>
       <c r="BF19" s="48"/>
     </row>
-    <row r="20" spans="2:58 16364:16364">
+    <row r="20" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B20" s="48"/>
       <c r="C20" s="3" t="s">
         <v>75</v>
@@ -3295,23 +3368,23 @@
       <c r="AO20" s="38"/>
       <c r="AP20" s="6"/>
       <c r="AQ20" s="48"/>
-      <c r="AR20" s="6"/>
-      <c r="AS20" s="6"/>
+      <c r="AR20" s="53"/>
+      <c r="AS20" s="52"/>
       <c r="AT20" s="6"/>
       <c r="AU20" s="6"/>
-      <c r="AV20" s="52"/>
-      <c r="AW20" s="52"/>
-      <c r="AX20" s="52"/>
-      <c r="AY20" s="6"/>
-      <c r="AZ20" s="6"/>
+      <c r="AV20" s="6"/>
+      <c r="AW20" s="66"/>
+      <c r="AX20" s="66"/>
+      <c r="AY20" s="66"/>
+      <c r="AZ20" s="52"/>
       <c r="BA20" s="6"/>
       <c r="BB20" s="6"/>
-      <c r="BC20" s="53"/>
-      <c r="BD20" s="52"/>
+      <c r="BC20" s="6"/>
+      <c r="BD20" s="6"/>
       <c r="BE20" s="6"/>
       <c r="BF20" s="48"/>
     </row>
-    <row r="21" spans="2:58 16364:16364" ht="8" customHeight="1">
+    <row r="21" spans="2:58 16364:16364" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="48"/>
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
@@ -3370,7 +3443,7 @@
       <c r="BE21" s="14"/>
       <c r="BF21" s="48"/>
     </row>
-    <row r="22" spans="2:58 16364:16364">
+    <row r="22" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B22" s="48"/>
       <c r="C22" s="3" t="s">
         <v>76</v>
@@ -3419,23 +3492,23 @@
       <c r="AO22" s="38"/>
       <c r="AP22" s="6"/>
       <c r="AQ22" s="48"/>
-      <c r="AR22" s="6"/>
-      <c r="AS22" s="6"/>
+      <c r="AR22" s="66"/>
+      <c r="AS22" s="52"/>
       <c r="AT22" s="6"/>
       <c r="AU22" s="6"/>
-      <c r="AV22" s="52"/>
-      <c r="AW22" s="52"/>
-      <c r="AX22" s="52"/>
-      <c r="AY22" s="6"/>
-      <c r="AZ22" s="6"/>
+      <c r="AV22" s="6"/>
+      <c r="AW22" s="6"/>
+      <c r="AX22" s="66"/>
+      <c r="AY22" s="53"/>
+      <c r="AZ22" s="52"/>
       <c r="BA22" s="6"/>
       <c r="BB22" s="6"/>
-      <c r="BC22" s="53"/>
-      <c r="BD22" s="52"/>
+      <c r="BC22" s="6"/>
+      <c r="BD22" s="6"/>
       <c r="BE22" s="6"/>
       <c r="BF22" s="48"/>
     </row>
-    <row r="23" spans="2:58 16364:16364">
+    <row r="23" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B23" s="48"/>
       <c r="C23" s="3" t="s">
         <v>77</v>
@@ -3484,23 +3557,23 @@
       <c r="AO23" s="38"/>
       <c r="AP23" s="6"/>
       <c r="AQ23" s="48"/>
-      <c r="AR23" s="6"/>
-      <c r="AS23" s="6"/>
+      <c r="AR23" s="66"/>
+      <c r="AS23" s="52"/>
       <c r="AT23" s="6"/>
       <c r="AU23" s="6"/>
-      <c r="AV23" s="52"/>
-      <c r="AW23" s="52"/>
-      <c r="AX23" s="52"/>
-      <c r="AY23" s="6"/>
-      <c r="AZ23" s="6"/>
+      <c r="AV23" s="6"/>
+      <c r="AW23" s="66"/>
+      <c r="AX23" s="53"/>
+      <c r="AY23" s="52"/>
+      <c r="AZ23" s="52"/>
       <c r="BA23" s="6"/>
       <c r="BB23" s="6"/>
-      <c r="BC23" s="53"/>
-      <c r="BD23" s="52"/>
+      <c r="BC23" s="6"/>
+      <c r="BD23" s="6"/>
       <c r="BE23" s="6"/>
       <c r="BF23" s="48"/>
     </row>
-    <row r="24" spans="2:58 16364:16364">
+    <row r="24" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B24" s="48"/>
       <c r="C24" s="3" t="s">
         <v>78</v>
@@ -3512,44 +3585,44 @@
         <v>20</v>
       </c>
       <c r="F24" s="48"/>
-      <c r="G24" s="56" t="s">
+      <c r="G24" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="57"/>
-      <c r="S24" s="57"/>
-      <c r="T24" s="57"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="57"/>
-      <c r="W24" s="57"/>
-      <c r="X24" s="57"/>
-      <c r="Y24" s="57"/>
-      <c r="Z24" s="57"/>
-      <c r="AA24" s="57"/>
-      <c r="AB24" s="57"/>
-      <c r="AC24" s="57"/>
-      <c r="AD24" s="57"/>
-      <c r="AE24" s="57"/>
-      <c r="AF24" s="57"/>
-      <c r="AG24" s="57"/>
-      <c r="AH24" s="57"/>
-      <c r="AI24" s="57"/>
-      <c r="AJ24" s="57"/>
-      <c r="AK24" s="57"/>
-      <c r="AL24" s="57"/>
-      <c r="AM24" s="57"/>
-      <c r="AN24" s="57"/>
-      <c r="AO24" s="57"/>
-      <c r="AP24" s="58"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="61"/>
+      <c r="V24" s="61"/>
+      <c r="W24" s="61"/>
+      <c r="X24" s="61"/>
+      <c r="Y24" s="61"/>
+      <c r="Z24" s="61"/>
+      <c r="AA24" s="61"/>
+      <c r="AB24" s="61"/>
+      <c r="AC24" s="61"/>
+      <c r="AD24" s="61"/>
+      <c r="AE24" s="61"/>
+      <c r="AF24" s="61"/>
+      <c r="AG24" s="61"/>
+      <c r="AH24" s="61"/>
+      <c r="AI24" s="61"/>
+      <c r="AJ24" s="61"/>
+      <c r="AK24" s="61"/>
+      <c r="AL24" s="61"/>
+      <c r="AM24" s="61"/>
+      <c r="AN24" s="61"/>
+      <c r="AO24" s="61"/>
+      <c r="AP24" s="62"/>
       <c r="AQ24" s="48"/>
       <c r="AR24" s="51"/>
       <c r="AS24" s="51"/>
@@ -3567,7 +3640,7 @@
       <c r="BE24" s="51"/>
       <c r="BF24" s="48"/>
     </row>
-    <row r="25" spans="2:58 16364:16364">
+    <row r="25" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B25" s="48"/>
       <c r="C25" s="3" t="s">
         <v>79</v>
@@ -3579,44 +3652,44 @@
         <v>19</v>
       </c>
       <c r="F25" s="48"/>
-      <c r="G25" s="59" t="s">
+      <c r="G25" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="60"/>
-      <c r="W25" s="60"/>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="60"/>
-      <c r="Z25" s="60"/>
-      <c r="AA25" s="60"/>
-      <c r="AB25" s="60"/>
-      <c r="AC25" s="60"/>
-      <c r="AD25" s="60"/>
-      <c r="AE25" s="60"/>
-      <c r="AF25" s="60"/>
-      <c r="AG25" s="60"/>
-      <c r="AH25" s="60"/>
-      <c r="AI25" s="60"/>
-      <c r="AJ25" s="60"/>
-      <c r="AK25" s="60"/>
-      <c r="AL25" s="60"/>
-      <c r="AM25" s="60"/>
-      <c r="AN25" s="60"/>
-      <c r="AO25" s="60"/>
-      <c r="AP25" s="61"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="64"/>
+      <c r="S25" s="64"/>
+      <c r="T25" s="64"/>
+      <c r="U25" s="64"/>
+      <c r="V25" s="64"/>
+      <c r="W25" s="64"/>
+      <c r="X25" s="64"/>
+      <c r="Y25" s="64"/>
+      <c r="Z25" s="64"/>
+      <c r="AA25" s="64"/>
+      <c r="AB25" s="64"/>
+      <c r="AC25" s="64"/>
+      <c r="AD25" s="64"/>
+      <c r="AE25" s="64"/>
+      <c r="AF25" s="64"/>
+      <c r="AG25" s="64"/>
+      <c r="AH25" s="64"/>
+      <c r="AI25" s="64"/>
+      <c r="AJ25" s="64"/>
+      <c r="AK25" s="64"/>
+      <c r="AL25" s="64"/>
+      <c r="AM25" s="64"/>
+      <c r="AN25" s="64"/>
+      <c r="AO25" s="64"/>
+      <c r="AP25" s="65"/>
       <c r="AQ25" s="48"/>
       <c r="AR25" s="50"/>
       <c r="AS25" s="50"/>
@@ -3634,7 +3707,7 @@
       <c r="BE25" s="50"/>
       <c r="BF25" s="48"/>
     </row>
-    <row r="26" spans="2:58 16364:16364">
+    <row r="26" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B26" s="48"/>
       <c r="C26" s="3" t="s">
         <v>80</v>
@@ -3683,23 +3756,23 @@
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
       <c r="AQ26" s="48"/>
-      <c r="AR26" s="30"/>
+      <c r="AR26" s="6"/>
       <c r="AS26" s="6"/>
-      <c r="AT26" s="6"/>
+      <c r="AT26" s="53"/>
       <c r="AU26" s="6"/>
       <c r="AV26" s="6"/>
-      <c r="AW26" s="52"/>
-      <c r="AX26" s="52"/>
+      <c r="AW26" s="6"/>
+      <c r="AX26" s="6"/>
       <c r="AY26" s="52"/>
       <c r="AZ26" s="52"/>
-      <c r="BA26" s="6"/>
-      <c r="BB26" s="6"/>
+      <c r="BA26" s="52"/>
+      <c r="BB26" s="52"/>
       <c r="BC26" s="6"/>
       <c r="BD26" s="6"/>
       <c r="BE26" s="6"/>
       <c r="BF26" s="48"/>
     </row>
-    <row r="27" spans="2:58 16364:16364">
+    <row r="27" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B27" s="48"/>
       <c r="C27" s="3" t="s">
         <v>81</v>
@@ -3753,19 +3826,19 @@
       <c r="AT27" s="6"/>
       <c r="AU27" s="6"/>
       <c r="AV27" s="6"/>
-      <c r="AW27" s="6"/>
-      <c r="AX27" s="54"/>
-      <c r="AY27" s="54"/>
-      <c r="AZ27" s="53"/>
-      <c r="BA27" s="6"/>
-      <c r="BB27" s="6"/>
-      <c r="BC27" s="6"/>
-      <c r="BD27" s="6"/>
+      <c r="AW27" s="53"/>
+      <c r="AX27" s="6"/>
+      <c r="AY27" s="6"/>
+      <c r="AZ27" s="54"/>
+      <c r="BA27" s="54"/>
+      <c r="BB27" s="66"/>
+      <c r="BC27" s="66"/>
+      <c r="BD27" s="66"/>
       <c r="BE27" s="6"/>
       <c r="BF27" s="48"/>
       <c r="XEJ27" s="6"/>
     </row>
-    <row r="28" spans="2:58 16364:16364">
+    <row r="28" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B28" s="48"/>
       <c r="C28" s="3" t="s">
         <v>82</v>
@@ -3820,17 +3893,17 @@
       <c r="AU28" s="6"/>
       <c r="AV28" s="6"/>
       <c r="AW28" s="6"/>
-      <c r="AX28" s="54"/>
-      <c r="AY28" s="54"/>
-      <c r="AZ28" s="6"/>
-      <c r="BA28" s="53"/>
-      <c r="BB28" s="6"/>
-      <c r="BC28" s="6"/>
-      <c r="BD28" s="6"/>
+      <c r="AX28" s="6"/>
+      <c r="AY28" s="6"/>
+      <c r="AZ28" s="68"/>
+      <c r="BA28" s="54"/>
+      <c r="BB28" s="66"/>
+      <c r="BC28" s="66"/>
+      <c r="BD28" s="66"/>
       <c r="BE28" s="6"/>
       <c r="BF28" s="48"/>
     </row>
-    <row r="29" spans="2:58 16364:16364">
+    <row r="29" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B29" s="48"/>
       <c r="C29" s="3" t="s">
         <v>83</v>
@@ -3885,17 +3958,17 @@
       <c r="AU29" s="6"/>
       <c r="AV29" s="6"/>
       <c r="AW29" s="6"/>
-      <c r="AX29" s="54"/>
-      <c r="AY29" s="54"/>
-      <c r="AZ29" s="6"/>
-      <c r="BA29" s="6"/>
-      <c r="BB29" s="53"/>
-      <c r="BC29" s="6"/>
-      <c r="BD29" s="6"/>
+      <c r="AX29" s="6"/>
+      <c r="AY29" s="6"/>
+      <c r="AZ29" s="68"/>
+      <c r="BA29" s="54"/>
+      <c r="BB29" s="66"/>
+      <c r="BC29" s="66"/>
+      <c r="BD29" s="66"/>
       <c r="BE29" s="6"/>
       <c r="BF29" s="48"/>
     </row>
-    <row r="30" spans="2:58 16364:16364">
+    <row r="30" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B30" s="48"/>
       <c r="C30" s="3" t="s">
         <v>84</v>
@@ -3907,44 +3980,44 @@
         <v>9</v>
       </c>
       <c r="F30" s="48"/>
-      <c r="G30" s="59" t="s">
+      <c r="G30" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="60"/>
-      <c r="U30" s="60"/>
-      <c r="V30" s="60"/>
-      <c r="W30" s="60"/>
-      <c r="X30" s="60"/>
-      <c r="Y30" s="60"/>
-      <c r="Z30" s="60"/>
-      <c r="AA30" s="60"/>
-      <c r="AB30" s="60"/>
-      <c r="AC30" s="60"/>
-      <c r="AD30" s="60"/>
-      <c r="AE30" s="60"/>
-      <c r="AF30" s="60"/>
-      <c r="AG30" s="60"/>
-      <c r="AH30" s="60"/>
-      <c r="AI30" s="60"/>
-      <c r="AJ30" s="60"/>
-      <c r="AK30" s="60"/>
-      <c r="AL30" s="60"/>
-      <c r="AM30" s="60"/>
-      <c r="AN30" s="60"/>
-      <c r="AO30" s="60"/>
-      <c r="AP30" s="61"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="64"/>
+      <c r="Q30" s="64"/>
+      <c r="R30" s="64"/>
+      <c r="S30" s="64"/>
+      <c r="T30" s="64"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="64"/>
+      <c r="W30" s="64"/>
+      <c r="X30" s="64"/>
+      <c r="Y30" s="64"/>
+      <c r="Z30" s="64"/>
+      <c r="AA30" s="64"/>
+      <c r="AB30" s="64"/>
+      <c r="AC30" s="64"/>
+      <c r="AD30" s="64"/>
+      <c r="AE30" s="64"/>
+      <c r="AF30" s="64"/>
+      <c r="AG30" s="64"/>
+      <c r="AH30" s="64"/>
+      <c r="AI30" s="64"/>
+      <c r="AJ30" s="64"/>
+      <c r="AK30" s="64"/>
+      <c r="AL30" s="64"/>
+      <c r="AM30" s="64"/>
+      <c r="AN30" s="64"/>
+      <c r="AO30" s="64"/>
+      <c r="AP30" s="65"/>
       <c r="AQ30" s="48"/>
       <c r="AR30" s="50"/>
       <c r="AS30" s="50"/>
@@ -3962,7 +4035,7 @@
       <c r="BE30" s="50"/>
       <c r="BF30" s="48"/>
     </row>
-    <row r="31" spans="2:58 16364:16364">
+    <row r="31" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B31" s="48"/>
       <c r="C31" s="3" t="s">
         <v>85</v>
@@ -3974,44 +4047,44 @@
         <v>10</v>
       </c>
       <c r="F31" s="48"/>
-      <c r="G31" s="56" t="s">
+      <c r="G31" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="57"/>
-      <c r="R31" s="57"/>
-      <c r="S31" s="57"/>
-      <c r="T31" s="57"/>
-      <c r="U31" s="57"/>
-      <c r="V31" s="57"/>
-      <c r="W31" s="57"/>
-      <c r="X31" s="57"/>
-      <c r="Y31" s="57"/>
-      <c r="Z31" s="57"/>
-      <c r="AA31" s="57"/>
-      <c r="AB31" s="57"/>
-      <c r="AC31" s="57"/>
-      <c r="AD31" s="57"/>
-      <c r="AE31" s="57"/>
-      <c r="AF31" s="57"/>
-      <c r="AG31" s="57"/>
-      <c r="AH31" s="57"/>
-      <c r="AI31" s="57"/>
-      <c r="AJ31" s="57"/>
-      <c r="AK31" s="57"/>
-      <c r="AL31" s="57"/>
-      <c r="AM31" s="57"/>
-      <c r="AN31" s="57"/>
-      <c r="AO31" s="57"/>
-      <c r="AP31" s="58"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="61"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="61"/>
+      <c r="S31" s="61"/>
+      <c r="T31" s="61"/>
+      <c r="U31" s="61"/>
+      <c r="V31" s="61"/>
+      <c r="W31" s="61"/>
+      <c r="X31" s="61"/>
+      <c r="Y31" s="61"/>
+      <c r="Z31" s="61"/>
+      <c r="AA31" s="61"/>
+      <c r="AB31" s="61"/>
+      <c r="AC31" s="61"/>
+      <c r="AD31" s="61"/>
+      <c r="AE31" s="61"/>
+      <c r="AF31" s="61"/>
+      <c r="AG31" s="61"/>
+      <c r="AH31" s="61"/>
+      <c r="AI31" s="61"/>
+      <c r="AJ31" s="61"/>
+      <c r="AK31" s="61"/>
+      <c r="AL31" s="61"/>
+      <c r="AM31" s="61"/>
+      <c r="AN31" s="61"/>
+      <c r="AO31" s="61"/>
+      <c r="AP31" s="62"/>
       <c r="AQ31" s="48"/>
       <c r="AR31" s="51"/>
       <c r="AS31" s="51"/>
@@ -4029,7 +4102,7 @@
       <c r="BE31" s="51"/>
       <c r="BF31" s="48"/>
     </row>
-    <row r="32" spans="2:58 16364:16364">
+    <row r="32" spans="2:58 16364:16364" x14ac:dyDescent="0.25">
       <c r="B32" s="48"/>
       <c r="C32" s="3" t="s">
         <v>86</v>
@@ -4079,22 +4152,22 @@
       <c r="AP32" s="6"/>
       <c r="AQ32" s="48"/>
       <c r="AR32" s="6"/>
-      <c r="AS32" s="6"/>
+      <c r="AS32" s="66"/>
       <c r="AT32" s="6"/>
       <c r="AU32" s="6"/>
       <c r="AV32" s="6"/>
       <c r="AW32" s="6"/>
-      <c r="AX32" s="52"/>
+      <c r="AX32" s="6"/>
       <c r="AY32" s="6"/>
-      <c r="AZ32" s="6"/>
+      <c r="AZ32" s="53"/>
       <c r="BA32" s="6"/>
       <c r="BB32" s="6"/>
       <c r="BC32" s="6"/>
       <c r="BD32" s="6"/>
-      <c r="BE32" s="30"/>
+      <c r="BE32" s="66"/>
       <c r="BF32" s="48"/>
     </row>
-    <row r="33" spans="2:58">
+    <row r="33" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B33" s="48"/>
       <c r="C33" s="3" t="s">
         <v>87</v>
@@ -4144,22 +4217,22 @@
       <c r="AP33" s="6"/>
       <c r="AQ33" s="48"/>
       <c r="AR33" s="6"/>
-      <c r="AS33" s="6"/>
+      <c r="AS33" s="66"/>
       <c r="AT33" s="6"/>
       <c r="AU33" s="6"/>
       <c r="AV33" s="6"/>
       <c r="AW33" s="6"/>
-      <c r="AX33" s="52"/>
+      <c r="AX33" s="6"/>
       <c r="AY33" s="6"/>
-      <c r="AZ33" s="6"/>
+      <c r="AZ33" s="53"/>
       <c r="BA33" s="6"/>
       <c r="BB33" s="6"/>
       <c r="BC33" s="6"/>
       <c r="BD33" s="6"/>
-      <c r="BE33" s="30"/>
+      <c r="BE33" s="66"/>
       <c r="BF33" s="48"/>
     </row>
-    <row r="34" spans="2:58">
+    <row r="34" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B34" s="48"/>
       <c r="C34" s="3" t="s">
         <v>88</v>
@@ -4208,23 +4281,23 @@
       <c r="AO34" s="6"/>
       <c r="AP34" s="6"/>
       <c r="AQ34" s="48"/>
-      <c r="AR34" s="30"/>
+      <c r="AR34" s="6"/>
       <c r="AS34" s="6"/>
-      <c r="AT34" s="6"/>
+      <c r="AT34" s="66"/>
       <c r="AU34" s="6"/>
       <c r="AV34" s="6"/>
-      <c r="AW34" s="52"/>
-      <c r="AX34" s="52"/>
+      <c r="AW34" s="6"/>
+      <c r="AX34" s="6"/>
       <c r="AY34" s="52"/>
-      <c r="AZ34" s="6"/>
-      <c r="BA34" s="6"/>
+      <c r="AZ34" s="53"/>
+      <c r="BA34" s="52"/>
       <c r="BB34" s="6"/>
       <c r="BC34" s="6"/>
       <c r="BD34" s="6"/>
       <c r="BE34" s="6"/>
       <c r="BF34" s="48"/>
     </row>
-    <row r="35" spans="2:58">
+    <row r="35" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B35" s="48"/>
       <c r="C35" s="3" t="s">
         <v>89</v>
@@ -4279,17 +4352,17 @@
       <c r="AU35" s="6"/>
       <c r="AV35" s="6"/>
       <c r="AW35" s="6"/>
-      <c r="AX35" s="30"/>
-      <c r="AY35" s="6"/>
-      <c r="AZ35" s="6"/>
-      <c r="BA35" s="6"/>
+      <c r="AX35" s="6"/>
+      <c r="AY35" s="66"/>
+      <c r="AZ35" s="53"/>
+      <c r="BA35" s="66"/>
       <c r="BB35" s="6"/>
       <c r="BC35" s="6"/>
       <c r="BD35" s="6"/>
       <c r="BE35" s="6"/>
       <c r="BF35" s="48"/>
     </row>
-    <row r="36" spans="2:58">
+    <row r="36" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B36" s="48"/>
       <c r="C36" s="3" t="s">
         <v>90</v>
@@ -4343,18 +4416,18 @@
       <c r="AT36" s="6"/>
       <c r="AU36" s="6"/>
       <c r="AV36" s="6"/>
-      <c r="AW36" s="6"/>
-      <c r="AX36" s="30"/>
-      <c r="AY36" s="6"/>
-      <c r="AZ36" s="6"/>
-      <c r="BA36" s="6"/>
+      <c r="AW36" s="66"/>
+      <c r="AX36" s="66"/>
+      <c r="AY36" s="66"/>
+      <c r="AZ36" s="66"/>
+      <c r="BA36" s="66"/>
       <c r="BB36" s="6"/>
       <c r="BC36" s="6"/>
       <c r="BD36" s="6"/>
       <c r="BE36" s="6"/>
       <c r="BF36" s="48"/>
     </row>
-    <row r="37" spans="2:58">
+    <row r="37" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B37" s="48"/>
       <c r="C37" s="3" t="s">
         <v>91</v>
@@ -4408,18 +4481,18 @@
       <c r="AT37" s="6"/>
       <c r="AU37" s="6"/>
       <c r="AV37" s="6"/>
-      <c r="AW37" s="6"/>
-      <c r="AX37" s="30"/>
-      <c r="AY37" s="6"/>
-      <c r="AZ37" s="6"/>
-      <c r="BA37" s="6"/>
+      <c r="AW37" s="66"/>
+      <c r="AX37" s="66"/>
+      <c r="AY37" s="66"/>
+      <c r="AZ37" s="66"/>
+      <c r="BA37" s="66"/>
       <c r="BB37" s="6"/>
       <c r="BC37" s="6"/>
       <c r="BD37" s="6"/>
       <c r="BE37" s="6"/>
       <c r="BF37" s="48"/>
     </row>
-    <row r="38" spans="2:58" ht="8" customHeight="1">
+    <row r="38" spans="2:58" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="48"/>
       <c r="C38" s="11"/>
       <c r="D38" s="12"/>
@@ -4478,7 +4551,7 @@
       <c r="BE38" s="14"/>
       <c r="BF38" s="48"/>
     </row>
-    <row r="39" spans="2:58">
+    <row r="39" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B39" s="48"/>
       <c r="C39" s="3" t="s">
         <v>92</v>
@@ -4527,23 +4600,23 @@
       <c r="AO39" s="10"/>
       <c r="AP39" s="10"/>
       <c r="AQ39" s="48"/>
-      <c r="AR39" s="6"/>
-      <c r="AS39" s="6"/>
+      <c r="AR39" s="52"/>
+      <c r="AS39" s="52"/>
       <c r="AT39" s="6"/>
       <c r="AU39" s="6"/>
       <c r="AV39" s="6"/>
       <c r="AW39" s="6"/>
-      <c r="AX39" s="30"/>
-      <c r="AY39" s="52"/>
-      <c r="AZ39" s="52"/>
-      <c r="BA39" s="52"/>
+      <c r="AX39" s="66"/>
+      <c r="AY39" s="66"/>
+      <c r="AZ39" s="66"/>
+      <c r="BA39" s="66"/>
       <c r="BB39" s="52"/>
       <c r="BC39" s="52"/>
       <c r="BD39" s="52"/>
       <c r="BE39" s="52"/>
       <c r="BF39" s="48"/>
     </row>
-    <row r="40" spans="2:58">
+    <row r="40" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B40" s="48"/>
       <c r="C40" s="3" t="s">
         <v>93</v>
@@ -4592,23 +4665,23 @@
       <c r="AO40" s="21"/>
       <c r="AP40" s="21"/>
       <c r="AQ40" s="48"/>
-      <c r="AR40" s="6"/>
-      <c r="AS40" s="6"/>
+      <c r="AR40" s="52"/>
+      <c r="AS40" s="52"/>
       <c r="AT40" s="6"/>
       <c r="AU40" s="6"/>
       <c r="AV40" s="6"/>
       <c r="AW40" s="6"/>
       <c r="AX40" s="6"/>
-      <c r="AY40" s="52"/>
-      <c r="AZ40" s="52"/>
-      <c r="BA40" s="52"/>
+      <c r="AY40" s="66"/>
+      <c r="AZ40" s="66"/>
+      <c r="BA40" s="66"/>
       <c r="BB40" s="52"/>
       <c r="BC40" s="52"/>
       <c r="BD40" s="52"/>
       <c r="BE40" s="52"/>
       <c r="BF40" s="48"/>
     </row>
-    <row r="41" spans="2:58">
+    <row r="41" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B41" s="48"/>
       <c r="C41" s="3" t="s">
         <v>110</v>
@@ -4657,23 +4730,23 @@
       <c r="AO41" s="21"/>
       <c r="AP41" s="21"/>
       <c r="AQ41" s="48"/>
-      <c r="AR41" s="6"/>
-      <c r="AS41" s="6"/>
+      <c r="AR41" s="52"/>
+      <c r="AS41" s="52"/>
       <c r="AT41" s="6"/>
       <c r="AU41" s="6"/>
       <c r="AV41" s="6"/>
       <c r="AW41" s="6"/>
-      <c r="AX41" s="6"/>
-      <c r="AY41" s="52"/>
-      <c r="AZ41" s="52"/>
-      <c r="BA41" s="52"/>
+      <c r="AX41" s="66"/>
+      <c r="AY41" s="66"/>
+      <c r="AZ41" s="66"/>
+      <c r="BA41" s="66"/>
       <c r="BB41" s="52"/>
       <c r="BC41" s="52"/>
       <c r="BD41" s="52"/>
       <c r="BE41" s="52"/>
       <c r="BF41" s="48"/>
     </row>
-    <row r="42" spans="2:58">
+    <row r="42" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B42" s="48"/>
       <c r="C42" s="3" t="s">
         <v>111</v>
@@ -4722,23 +4795,23 @@
       <c r="AO42" s="21"/>
       <c r="AP42" s="21"/>
       <c r="AQ42" s="48"/>
-      <c r="AR42" s="6"/>
-      <c r="AS42" s="6"/>
+      <c r="AR42" s="52"/>
+      <c r="AS42" s="52"/>
       <c r="AT42" s="6"/>
       <c r="AU42" s="6"/>
       <c r="AV42" s="6"/>
-      <c r="AW42" s="6"/>
-      <c r="AX42" s="30"/>
-      <c r="AY42" s="52"/>
-      <c r="AZ42" s="52"/>
-      <c r="BA42" s="52"/>
+      <c r="AW42" s="66"/>
+      <c r="AX42" s="6"/>
+      <c r="AY42" s="66"/>
+      <c r="AZ42" s="66"/>
+      <c r="BA42" s="66"/>
       <c r="BB42" s="52"/>
       <c r="BC42" s="52"/>
       <c r="BD42" s="52"/>
       <c r="BE42" s="52"/>
       <c r="BF42" s="48"/>
     </row>
-    <row r="43" spans="2:58">
+    <row r="43" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B43" s="48"/>
       <c r="C43" s="3" t="s">
         <v>112</v>
@@ -4787,23 +4860,23 @@
       <c r="AO43" s="21"/>
       <c r="AP43" s="21"/>
       <c r="AQ43" s="48"/>
-      <c r="AR43" s="6"/>
-      <c r="AS43" s="6"/>
+      <c r="AR43" s="52"/>
+      <c r="AS43" s="52"/>
       <c r="AT43" s="6"/>
       <c r="AU43" s="6"/>
       <c r="AV43" s="6"/>
-      <c r="AW43" s="6"/>
-      <c r="AX43" s="30"/>
-      <c r="AY43" s="52"/>
-      <c r="AZ43" s="52"/>
-      <c r="BA43" s="52"/>
+      <c r="AW43" s="66"/>
+      <c r="AX43" s="6"/>
+      <c r="AY43" s="66"/>
+      <c r="AZ43" s="66"/>
+      <c r="BA43" s="66"/>
       <c r="BB43" s="52"/>
       <c r="BC43" s="52"/>
       <c r="BD43" s="52"/>
       <c r="BE43" s="52"/>
       <c r="BF43" s="48"/>
     </row>
-    <row r="44" spans="2:58">
+    <row r="44" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B44" s="48"/>
       <c r="C44" s="3" t="s">
         <v>113</v>
@@ -4815,44 +4888,44 @@
         <v>10</v>
       </c>
       <c r="F44" s="48"/>
-      <c r="G44" s="56" t="s">
+      <c r="G44" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="57"/>
-      <c r="U44" s="57"/>
-      <c r="V44" s="57"/>
-      <c r="W44" s="57"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="57"/>
-      <c r="Z44" s="57"/>
-      <c r="AA44" s="57"/>
-      <c r="AB44" s="57"/>
-      <c r="AC44" s="57"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="57"/>
-      <c r="AF44" s="57"/>
-      <c r="AG44" s="57"/>
-      <c r="AH44" s="57"/>
-      <c r="AI44" s="57"/>
-      <c r="AJ44" s="57"/>
-      <c r="AK44" s="57"/>
-      <c r="AL44" s="57"/>
-      <c r="AM44" s="57"/>
-      <c r="AN44" s="57"/>
-      <c r="AO44" s="57"/>
-      <c r="AP44" s="58"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="61"/>
+      <c r="O44" s="61"/>
+      <c r="P44" s="61"/>
+      <c r="Q44" s="61"/>
+      <c r="R44" s="61"/>
+      <c r="S44" s="61"/>
+      <c r="T44" s="61"/>
+      <c r="U44" s="61"/>
+      <c r="V44" s="61"/>
+      <c r="W44" s="61"/>
+      <c r="X44" s="61"/>
+      <c r="Y44" s="61"/>
+      <c r="Z44" s="61"/>
+      <c r="AA44" s="61"/>
+      <c r="AB44" s="61"/>
+      <c r="AC44" s="61"/>
+      <c r="AD44" s="61"/>
+      <c r="AE44" s="61"/>
+      <c r="AF44" s="61"/>
+      <c r="AG44" s="61"/>
+      <c r="AH44" s="61"/>
+      <c r="AI44" s="61"/>
+      <c r="AJ44" s="61"/>
+      <c r="AK44" s="61"/>
+      <c r="AL44" s="61"/>
+      <c r="AM44" s="61"/>
+      <c r="AN44" s="61"/>
+      <c r="AO44" s="61"/>
+      <c r="AP44" s="62"/>
       <c r="AQ44" s="48"/>
       <c r="AR44" s="51"/>
       <c r="AS44" s="51"/>
@@ -4870,7 +4943,7 @@
       <c r="BE44" s="51"/>
       <c r="BF44" s="48"/>
     </row>
-    <row r="45" spans="2:58">
+    <row r="45" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B45" s="48"/>
       <c r="C45" s="3" t="s">
         <v>114</v>
@@ -4920,22 +4993,22 @@
       <c r="AP45" s="21"/>
       <c r="AQ45" s="48"/>
       <c r="AR45" s="6"/>
-      <c r="AS45" s="6"/>
+      <c r="AS45" s="30"/>
       <c r="AT45" s="6"/>
       <c r="AU45" s="6"/>
       <c r="AV45" s="6"/>
-      <c r="AW45" s="52"/>
+      <c r="AW45" s="6"/>
       <c r="AX45" s="6"/>
-      <c r="AY45" s="6"/>
+      <c r="AY45" s="52"/>
       <c r="AZ45" s="6"/>
       <c r="BA45" s="6"/>
       <c r="BB45" s="6"/>
       <c r="BC45" s="6"/>
-      <c r="BD45" s="30"/>
+      <c r="BD45" s="6"/>
       <c r="BE45" s="6"/>
       <c r="BF45" s="48"/>
     </row>
-    <row r="46" spans="2:58">
+    <row r="46" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B46" s="48"/>
       <c r="C46" s="3" t="s">
         <v>115</v>
@@ -4985,22 +5058,22 @@
       <c r="AP46" s="21"/>
       <c r="AQ46" s="48"/>
       <c r="AR46" s="6"/>
-      <c r="AS46" s="6"/>
+      <c r="AS46" s="30"/>
       <c r="AT46" s="6"/>
       <c r="AU46" s="6"/>
       <c r="AV46" s="6"/>
-      <c r="AW46" s="52"/>
+      <c r="AW46" s="6"/>
       <c r="AX46" s="6"/>
-      <c r="AY46" s="6"/>
+      <c r="AY46" s="52"/>
       <c r="AZ46" s="6"/>
       <c r="BA46" s="6"/>
       <c r="BB46" s="6"/>
       <c r="BC46" s="6"/>
-      <c r="BD46" s="30"/>
+      <c r="BD46" s="6"/>
       <c r="BE46" s="6"/>
       <c r="BF46" s="48"/>
     </row>
-    <row r="47" spans="2:58">
+    <row r="47" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B47" s="48"/>
       <c r="C47" s="3" t="s">
         <v>116</v>
@@ -5012,44 +5085,44 @@
         <v>9</v>
       </c>
       <c r="F47" s="48"/>
-      <c r="G47" s="59" t="s">
+      <c r="G47" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="60"/>
-      <c r="N47" s="60"/>
-      <c r="O47" s="60"/>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="60"/>
-      <c r="R47" s="60"/>
-      <c r="S47" s="60"/>
-      <c r="T47" s="60"/>
-      <c r="U47" s="60"/>
-      <c r="V47" s="60"/>
-      <c r="W47" s="60"/>
-      <c r="X47" s="60"/>
-      <c r="Y47" s="60"/>
-      <c r="Z47" s="60"/>
-      <c r="AA47" s="60"/>
-      <c r="AB47" s="60"/>
-      <c r="AC47" s="60"/>
-      <c r="AD47" s="60"/>
-      <c r="AE47" s="60"/>
-      <c r="AF47" s="60"/>
-      <c r="AG47" s="60"/>
-      <c r="AH47" s="60"/>
-      <c r="AI47" s="60"/>
-      <c r="AJ47" s="60"/>
-      <c r="AK47" s="60"/>
-      <c r="AL47" s="60"/>
-      <c r="AM47" s="60"/>
-      <c r="AN47" s="60"/>
-      <c r="AO47" s="60"/>
-      <c r="AP47" s="61"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="64"/>
+      <c r="N47" s="64"/>
+      <c r="O47" s="64"/>
+      <c r="P47" s="64"/>
+      <c r="Q47" s="64"/>
+      <c r="R47" s="64"/>
+      <c r="S47" s="64"/>
+      <c r="T47" s="64"/>
+      <c r="U47" s="64"/>
+      <c r="V47" s="64"/>
+      <c r="W47" s="64"/>
+      <c r="X47" s="64"/>
+      <c r="Y47" s="64"/>
+      <c r="Z47" s="64"/>
+      <c r="AA47" s="64"/>
+      <c r="AB47" s="64"/>
+      <c r="AC47" s="64"/>
+      <c r="AD47" s="64"/>
+      <c r="AE47" s="64"/>
+      <c r="AF47" s="64"/>
+      <c r="AG47" s="64"/>
+      <c r="AH47" s="64"/>
+      <c r="AI47" s="64"/>
+      <c r="AJ47" s="64"/>
+      <c r="AK47" s="64"/>
+      <c r="AL47" s="64"/>
+      <c r="AM47" s="64"/>
+      <c r="AN47" s="64"/>
+      <c r="AO47" s="64"/>
+      <c r="AP47" s="65"/>
       <c r="AQ47" s="48"/>
       <c r="AR47" s="50"/>
       <c r="AS47" s="50"/>
@@ -5067,7 +5140,7 @@
       <c r="BE47" s="50"/>
       <c r="BF47" s="48"/>
     </row>
-    <row r="48" spans="2:58">
+    <row r="48" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B48" s="48"/>
       <c r="C48" s="3" t="s">
         <v>117</v>
@@ -5120,10 +5193,10 @@
       <c r="AS48" s="6"/>
       <c r="AT48" s="6"/>
       <c r="AU48" s="6"/>
-      <c r="AV48" s="30"/>
-      <c r="AW48" s="6"/>
-      <c r="AX48" s="6"/>
-      <c r="AY48" s="6"/>
+      <c r="AV48" s="6"/>
+      <c r="AW48" s="66"/>
+      <c r="AX48" s="66"/>
+      <c r="AY48" s="66"/>
       <c r="AZ48" s="6"/>
       <c r="BA48" s="6"/>
       <c r="BB48" s="6"/>
@@ -5132,7 +5205,7 @@
       <c r="BE48" s="6"/>
       <c r="BF48" s="48"/>
     </row>
-    <row r="49" spans="2:58">
+    <row r="49" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B49" s="48"/>
       <c r="C49" s="3" t="s">
         <v>118</v>
@@ -5183,12 +5256,12 @@
       <c r="AQ49" s="48"/>
       <c r="AR49" s="6"/>
       <c r="AS49" s="6"/>
-      <c r="AT49" s="6"/>
+      <c r="AT49" s="66"/>
       <c r="AU49" s="6"/>
-      <c r="AV49" s="30"/>
-      <c r="AW49" s="6"/>
-      <c r="AX49" s="6"/>
-      <c r="AY49" s="6"/>
+      <c r="AV49" s="6"/>
+      <c r="AW49" s="66"/>
+      <c r="AX49" s="66"/>
+      <c r="AY49" s="66"/>
       <c r="AZ49" s="6"/>
       <c r="BA49" s="6"/>
       <c r="BB49" s="6"/>
@@ -5197,7 +5270,7 @@
       <c r="BE49" s="6"/>
       <c r="BF49" s="48"/>
     </row>
-    <row r="50" spans="2:58">
+    <row r="50" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B50" s="48"/>
       <c r="C50" s="3" t="s">
         <v>119</v>
@@ -5250,10 +5323,10 @@
       <c r="AS50" s="6"/>
       <c r="AT50" s="6"/>
       <c r="AU50" s="6"/>
-      <c r="AV50" s="30"/>
-      <c r="AW50" s="6"/>
-      <c r="AX50" s="6"/>
-      <c r="AY50" s="6"/>
+      <c r="AV50" s="6"/>
+      <c r="AW50" s="66"/>
+      <c r="AX50" s="66"/>
+      <c r="AY50" s="66"/>
       <c r="AZ50" s="6"/>
       <c r="BA50" s="6"/>
       <c r="BB50" s="6"/>
@@ -5262,7 +5335,7 @@
       <c r="BE50" s="6"/>
       <c r="BF50" s="48"/>
     </row>
-    <row r="51" spans="2:58">
+    <row r="51" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B51" s="48"/>
       <c r="C51" s="3" t="s">
         <v>120</v>
@@ -5315,10 +5388,10 @@
       <c r="AS51" s="6"/>
       <c r="AT51" s="6"/>
       <c r="AU51" s="6"/>
-      <c r="AV51" s="30"/>
-      <c r="AW51" s="6"/>
-      <c r="AX51" s="6"/>
-      <c r="AY51" s="6"/>
+      <c r="AV51" s="6"/>
+      <c r="AW51" s="66"/>
+      <c r="AX51" s="66"/>
+      <c r="AY51" s="66"/>
       <c r="AZ51" s="6"/>
       <c r="BA51" s="6"/>
       <c r="BB51" s="6"/>
@@ -5327,7 +5400,7 @@
       <c r="BE51" s="6"/>
       <c r="BF51" s="48"/>
     </row>
-    <row r="52" spans="2:58">
+    <row r="52" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B52" s="48"/>
       <c r="C52" s="3" t="s">
         <v>121</v>
@@ -5380,19 +5453,19 @@
       <c r="AS52" s="6"/>
       <c r="AT52" s="6"/>
       <c r="AU52" s="6"/>
-      <c r="AV52" s="30"/>
-      <c r="AW52" s="52"/>
-      <c r="AX52" s="6"/>
-      <c r="AY52" s="6"/>
+      <c r="AV52" s="6"/>
+      <c r="AW52" s="66"/>
+      <c r="AX52" s="66"/>
+      <c r="AY52" s="66"/>
       <c r="AZ52" s="6"/>
       <c r="BA52" s="6"/>
       <c r="BB52" s="6"/>
       <c r="BC52" s="6"/>
-      <c r="BD52" s="6"/>
+      <c r="BD52" s="53"/>
       <c r="BE52" s="6"/>
       <c r="BF52" s="48"/>
     </row>
-    <row r="53" spans="2:58">
+    <row r="53" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B53" s="48"/>
       <c r="C53" s="3" t="s">
         <v>122</v>
@@ -5446,18 +5519,18 @@
       <c r="AT53" s="6"/>
       <c r="AU53" s="6"/>
       <c r="AV53" s="6"/>
-      <c r="AW53" s="52"/>
+      <c r="AW53" s="6"/>
       <c r="AX53" s="6"/>
-      <c r="AY53" s="6"/>
+      <c r="AY53" s="52"/>
       <c r="AZ53" s="6"/>
-      <c r="BA53" s="6"/>
+      <c r="BA53" s="53"/>
       <c r="BB53" s="6"/>
       <c r="BC53" s="6"/>
       <c r="BD53" s="6"/>
       <c r="BE53" s="6"/>
       <c r="BF53" s="48"/>
     </row>
-    <row r="54" spans="2:58">
+    <row r="54" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B54" s="48"/>
       <c r="C54" s="3" t="s">
         <v>123</v>
@@ -5511,18 +5584,18 @@
       <c r="AT54" s="6"/>
       <c r="AU54" s="6"/>
       <c r="AV54" s="6"/>
-      <c r="AW54" s="52"/>
+      <c r="AW54" s="6"/>
       <c r="AX54" s="6"/>
-      <c r="AY54" s="6"/>
+      <c r="AY54" s="52"/>
       <c r="AZ54" s="6"/>
-      <c r="BA54" s="6"/>
+      <c r="BA54" s="53"/>
       <c r="BB54" s="6"/>
       <c r="BC54" s="6"/>
       <c r="BD54" s="6"/>
       <c r="BE54" s="6"/>
       <c r="BF54" s="48"/>
     </row>
-    <row r="55" spans="2:58" ht="8" customHeight="1">
+    <row r="55" spans="2:58" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="48"/>
       <c r="C55" s="11"/>
       <c r="D55" s="12"/>
@@ -5581,7 +5654,7 @@
       <c r="BE55" s="55"/>
       <c r="BF55" s="48"/>
     </row>
-    <row r="56" spans="2:58">
+    <row r="56" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B56" s="48"/>
       <c r="C56" s="3" t="s">
         <v>94</v>
@@ -5633,20 +5706,20 @@
       <c r="AR56" s="6"/>
       <c r="AS56" s="6"/>
       <c r="AT56" s="6"/>
-      <c r="AU56" s="30"/>
-      <c r="AV56" s="6"/>
-      <c r="AW56" s="6"/>
-      <c r="AX56" s="6"/>
+      <c r="AU56" s="6"/>
+      <c r="AV56" s="66"/>
+      <c r="AW56" s="66"/>
+      <c r="AX56" s="66"/>
       <c r="AY56" s="6"/>
       <c r="AZ56" s="6"/>
       <c r="BA56" s="6"/>
       <c r="BB56" s="6"/>
-      <c r="BC56" s="6"/>
+      <c r="BC56" s="53"/>
       <c r="BD56" s="6"/>
       <c r="BE56" s="6"/>
       <c r="BF56" s="48"/>
     </row>
-    <row r="57" spans="2:58">
+    <row r="57" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B57" s="48"/>
       <c r="C57" s="3" t="s">
         <v>95</v>
@@ -5698,20 +5771,20 @@
       <c r="AR57" s="6"/>
       <c r="AS57" s="6"/>
       <c r="AT57" s="6"/>
-      <c r="AU57" s="30"/>
-      <c r="AV57" s="6"/>
-      <c r="AW57" s="6"/>
-      <c r="AX57" s="6"/>
+      <c r="AU57" s="6"/>
+      <c r="AV57" s="66"/>
+      <c r="AW57" s="66"/>
+      <c r="AX57" s="66"/>
       <c r="AY57" s="6"/>
       <c r="AZ57" s="6"/>
       <c r="BA57" s="6"/>
-      <c r="BB57" s="6"/>
+      <c r="BB57" s="53"/>
       <c r="BC57" s="6"/>
       <c r="BD57" s="6"/>
       <c r="BE57" s="6"/>
       <c r="BF57" s="48"/>
     </row>
-    <row r="58" spans="2:58">
+    <row r="58" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B58" s="48"/>
       <c r="C58" s="3" t="s">
         <v>96</v>
@@ -5763,10 +5836,10 @@
       <c r="AR58" s="6"/>
       <c r="AS58" s="6"/>
       <c r="AT58" s="6"/>
-      <c r="AU58" s="30"/>
-      <c r="AV58" s="6"/>
-      <c r="AW58" s="6"/>
-      <c r="AX58" s="6"/>
+      <c r="AU58" s="53"/>
+      <c r="AV58" s="66"/>
+      <c r="AW58" s="66"/>
+      <c r="AX58" s="66"/>
       <c r="AY58" s="6"/>
       <c r="AZ58" s="6"/>
       <c r="BA58" s="6"/>
@@ -5776,7 +5849,7 @@
       <c r="BE58" s="6"/>
       <c r="BF58" s="48"/>
     </row>
-    <row r="59" spans="2:58">
+    <row r="59" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B59" s="48"/>
       <c r="C59" s="3" t="s">
         <v>97</v>
@@ -5828,11 +5901,11 @@
       <c r="AR59" s="6"/>
       <c r="AS59" s="6"/>
       <c r="AT59" s="6"/>
-      <c r="AU59" s="30"/>
-      <c r="AV59" s="6"/>
-      <c r="AW59" s="6"/>
-      <c r="AX59" s="6"/>
-      <c r="AY59" s="6"/>
+      <c r="AU59" s="53"/>
+      <c r="AV59" s="66"/>
+      <c r="AW59" s="66"/>
+      <c r="AX59" s="66"/>
+      <c r="AY59" s="66"/>
       <c r="AZ59" s="6"/>
       <c r="BA59" s="6"/>
       <c r="BB59" s="6"/>
@@ -5841,7 +5914,7 @@
       <c r="BE59" s="6"/>
       <c r="BF59" s="48"/>
     </row>
-    <row r="60" spans="2:58">
+    <row r="60" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B60" s="47"/>
       <c r="C60" s="3" t="s">
         <v>98</v>
@@ -5893,12 +5966,12 @@
       <c r="AR60" s="6"/>
       <c r="AS60" s="6"/>
       <c r="AT60" s="6"/>
-      <c r="AU60" s="30"/>
-      <c r="AV60" s="6"/>
-      <c r="AW60" s="6"/>
-      <c r="AX60" s="6"/>
-      <c r="AY60" s="6"/>
-      <c r="AZ60" s="6"/>
+      <c r="AU60" s="66"/>
+      <c r="AV60" s="66"/>
+      <c r="AW60" s="53"/>
+      <c r="AX60" s="66"/>
+      <c r="AY60" s="66"/>
+      <c r="AZ60" s="66"/>
       <c r="BA60" s="6"/>
       <c r="BB60" s="6"/>
       <c r="BC60" s="6"/>
@@ -5906,7 +5979,7 @@
       <c r="BE60" s="6"/>
       <c r="BF60" s="47"/>
     </row>
-    <row r="61" spans="2:58">
+    <row r="61" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B61" s="47"/>
       <c r="C61" s="3" t="s">
         <v>99</v>
@@ -5958,12 +6031,12 @@
       <c r="AR61" s="6"/>
       <c r="AS61" s="6"/>
       <c r="AT61" s="6"/>
-      <c r="AU61" s="30"/>
-      <c r="AV61" s="6"/>
-      <c r="AW61" s="6"/>
-      <c r="AX61" s="6"/>
-      <c r="AY61" s="6"/>
-      <c r="AZ61" s="6"/>
+      <c r="AU61" s="66"/>
+      <c r="AV61" s="66"/>
+      <c r="AW61" s="53"/>
+      <c r="AX61" s="66"/>
+      <c r="AY61" s="66"/>
+      <c r="AZ61" s="66"/>
       <c r="BA61" s="6"/>
       <c r="BB61" s="6"/>
       <c r="BC61" s="6"/>
@@ -5971,7 +6044,7 @@
       <c r="BE61" s="6"/>
       <c r="BF61" s="47"/>
     </row>
-    <row r="62" spans="2:58">
+    <row r="62" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B62" s="47"/>
       <c r="C62" s="3" t="s">
         <v>100</v>
@@ -6023,12 +6096,12 @@
       <c r="AR62" s="6"/>
       <c r="AS62" s="6"/>
       <c r="AT62" s="6"/>
-      <c r="AU62" s="30"/>
-      <c r="AV62" s="6"/>
-      <c r="AW62" s="6"/>
-      <c r="AX62" s="6"/>
-      <c r="AY62" s="6"/>
-      <c r="AZ62" s="6"/>
+      <c r="AU62" s="66"/>
+      <c r="AV62" s="66"/>
+      <c r="AW62" s="53"/>
+      <c r="AX62" s="66"/>
+      <c r="AY62" s="66"/>
+      <c r="AZ62" s="66"/>
       <c r="BA62" s="6"/>
       <c r="BB62" s="6"/>
       <c r="BC62" s="6"/>
@@ -6036,7 +6109,7 @@
       <c r="BE62" s="6"/>
       <c r="BF62" s="47"/>
     </row>
-    <row r="63" spans="2:58">
+    <row r="63" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B63" s="47"/>
       <c r="C63" s="3" t="s">
         <v>101</v>
@@ -6048,44 +6121,44 @@
         <v>52</v>
       </c>
       <c r="F63" s="47"/>
-      <c r="G63" s="62" t="s">
+      <c r="G63" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="H63" s="63"/>
-      <c r="I63" s="63"/>
-      <c r="J63" s="63"/>
-      <c r="K63" s="63"/>
-      <c r="L63" s="63"/>
-      <c r="M63" s="63"/>
-      <c r="N63" s="63"/>
-      <c r="O63" s="63"/>
-      <c r="P63" s="63"/>
-      <c r="Q63" s="63"/>
-      <c r="R63" s="63"/>
-      <c r="S63" s="63"/>
-      <c r="T63" s="63"/>
-      <c r="U63" s="63"/>
-      <c r="V63" s="63"/>
-      <c r="W63" s="63"/>
-      <c r="X63" s="63"/>
-      <c r="Y63" s="63"/>
-      <c r="Z63" s="63"/>
-      <c r="AA63" s="63"/>
-      <c r="AB63" s="63"/>
-      <c r="AC63" s="63"/>
-      <c r="AD63" s="63"/>
-      <c r="AE63" s="63"/>
-      <c r="AF63" s="63"/>
-      <c r="AG63" s="63"/>
-      <c r="AH63" s="63"/>
-      <c r="AI63" s="63"/>
-      <c r="AJ63" s="63"/>
-      <c r="AK63" s="63"/>
-      <c r="AL63" s="63"/>
-      <c r="AM63" s="63"/>
-      <c r="AN63" s="63"/>
-      <c r="AO63" s="63"/>
-      <c r="AP63" s="64"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
+      <c r="J63" s="58"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="58"/>
+      <c r="O63" s="58"/>
+      <c r="P63" s="58"/>
+      <c r="Q63" s="58"/>
+      <c r="R63" s="58"/>
+      <c r="S63" s="58"/>
+      <c r="T63" s="58"/>
+      <c r="U63" s="58"/>
+      <c r="V63" s="58"/>
+      <c r="W63" s="58"/>
+      <c r="X63" s="58"/>
+      <c r="Y63" s="58"/>
+      <c r="Z63" s="58"/>
+      <c r="AA63" s="58"/>
+      <c r="AB63" s="58"/>
+      <c r="AC63" s="58"/>
+      <c r="AD63" s="58"/>
+      <c r="AE63" s="58"/>
+      <c r="AF63" s="58"/>
+      <c r="AG63" s="58"/>
+      <c r="AH63" s="58"/>
+      <c r="AI63" s="58"/>
+      <c r="AJ63" s="58"/>
+      <c r="AK63" s="58"/>
+      <c r="AL63" s="58"/>
+      <c r="AM63" s="58"/>
+      <c r="AN63" s="58"/>
+      <c r="AO63" s="58"/>
+      <c r="AP63" s="59"/>
       <c r="AQ63" s="47"/>
       <c r="AR63" s="49"/>
       <c r="AS63" s="49"/>
@@ -6103,7 +6176,7 @@
       <c r="BE63" s="49"/>
       <c r="BF63" s="47"/>
     </row>
-    <row r="64" spans="2:58">
+    <row r="64" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B64" s="47"/>
       <c r="C64" s="3" t="s">
         <v>102</v>
@@ -6115,44 +6188,44 @@
         <v>10</v>
       </c>
       <c r="F64" s="47"/>
-      <c r="G64" s="56" t="s">
+      <c r="G64" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
-      <c r="L64" s="57"/>
-      <c r="M64" s="57"/>
-      <c r="N64" s="57"/>
-      <c r="O64" s="57"/>
-      <c r="P64" s="57"/>
-      <c r="Q64" s="57"/>
-      <c r="R64" s="57"/>
-      <c r="S64" s="57"/>
-      <c r="T64" s="57"/>
-      <c r="U64" s="57"/>
-      <c r="V64" s="57"/>
-      <c r="W64" s="57"/>
-      <c r="X64" s="57"/>
-      <c r="Y64" s="57"/>
-      <c r="Z64" s="57"/>
-      <c r="AA64" s="57"/>
-      <c r="AB64" s="57"/>
-      <c r="AC64" s="57"/>
-      <c r="AD64" s="57"/>
-      <c r="AE64" s="57"/>
-      <c r="AF64" s="57"/>
-      <c r="AG64" s="57"/>
-      <c r="AH64" s="57"/>
-      <c r="AI64" s="57"/>
-      <c r="AJ64" s="57"/>
-      <c r="AK64" s="57"/>
-      <c r="AL64" s="57"/>
-      <c r="AM64" s="57"/>
-      <c r="AN64" s="57"/>
-      <c r="AO64" s="57"/>
-      <c r="AP64" s="58"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="61"/>
+      <c r="M64" s="61"/>
+      <c r="N64" s="61"/>
+      <c r="O64" s="61"/>
+      <c r="P64" s="61"/>
+      <c r="Q64" s="61"/>
+      <c r="R64" s="61"/>
+      <c r="S64" s="61"/>
+      <c r="T64" s="61"/>
+      <c r="U64" s="61"/>
+      <c r="V64" s="61"/>
+      <c r="W64" s="61"/>
+      <c r="X64" s="61"/>
+      <c r="Y64" s="61"/>
+      <c r="Z64" s="61"/>
+      <c r="AA64" s="61"/>
+      <c r="AB64" s="61"/>
+      <c r="AC64" s="61"/>
+      <c r="AD64" s="61"/>
+      <c r="AE64" s="61"/>
+      <c r="AF64" s="61"/>
+      <c r="AG64" s="61"/>
+      <c r="AH64" s="61"/>
+      <c r="AI64" s="61"/>
+      <c r="AJ64" s="61"/>
+      <c r="AK64" s="61"/>
+      <c r="AL64" s="61"/>
+      <c r="AM64" s="61"/>
+      <c r="AN64" s="61"/>
+      <c r="AO64" s="61"/>
+      <c r="AP64" s="62"/>
       <c r="AQ64" s="47"/>
       <c r="AR64" s="51"/>
       <c r="AS64" s="51"/>
@@ -6170,7 +6243,7 @@
       <c r="BE64" s="51"/>
       <c r="BF64" s="47"/>
     </row>
-    <row r="65" spans="2:58">
+    <row r="65" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B65" s="47"/>
       <c r="C65" s="3" t="s">
         <v>103</v>
@@ -6222,20 +6295,20 @@
       <c r="AR65" s="6"/>
       <c r="AS65" s="6"/>
       <c r="AT65" s="6"/>
-      <c r="AU65" s="6"/>
-      <c r="AV65" s="6"/>
-      <c r="AW65" s="6"/>
-      <c r="AX65" s="6"/>
-      <c r="AY65" s="30"/>
-      <c r="AZ65" s="6"/>
-      <c r="BA65" s="6"/>
-      <c r="BB65" s="6"/>
+      <c r="AU65" s="66"/>
+      <c r="AV65" s="66"/>
+      <c r="AW65" s="53"/>
+      <c r="AX65" s="66"/>
+      <c r="AY65" s="66"/>
+      <c r="AZ65" s="66"/>
+      <c r="BA65" s="66"/>
+      <c r="BB65" s="66"/>
       <c r="BC65" s="6"/>
       <c r="BD65" s="6"/>
       <c r="BE65" s="6"/>
       <c r="BF65" s="47"/>
     </row>
-    <row r="66" spans="2:58">
+    <row r="66" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B66" s="47"/>
       <c r="C66" s="3" t="s">
         <v>104</v>
@@ -6287,20 +6360,20 @@
       <c r="AR66" s="6"/>
       <c r="AS66" s="6"/>
       <c r="AT66" s="6"/>
-      <c r="AU66" s="6"/>
-      <c r="AV66" s="6"/>
-      <c r="AW66" s="6"/>
-      <c r="AX66" s="6"/>
-      <c r="AY66" s="30"/>
-      <c r="AZ66" s="6"/>
-      <c r="BA66" s="6"/>
-      <c r="BB66" s="6"/>
+      <c r="AU66" s="66"/>
+      <c r="AV66" s="66"/>
+      <c r="AW66" s="66"/>
+      <c r="AX66" s="53"/>
+      <c r="AY66" s="66"/>
+      <c r="AZ66" s="66"/>
+      <c r="BA66" s="66"/>
+      <c r="BB66" s="66"/>
       <c r="BC66" s="6"/>
       <c r="BD66" s="6"/>
       <c r="BE66" s="6"/>
       <c r="BF66" s="47"/>
     </row>
-    <row r="67" spans="2:58">
+    <row r="67" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B67" s="47"/>
       <c r="C67" s="3" t="s">
         <v>105</v>
@@ -6352,20 +6425,20 @@
       <c r="AR67" s="6"/>
       <c r="AS67" s="6"/>
       <c r="AT67" s="6"/>
-      <c r="AU67" s="30"/>
-      <c r="AV67" s="6"/>
-      <c r="AW67" s="6"/>
-      <c r="AX67" s="6"/>
-      <c r="AY67" s="6"/>
-      <c r="AZ67" s="6"/>
-      <c r="BA67" s="6"/>
+      <c r="AU67" s="66"/>
+      <c r="AV67" s="66"/>
+      <c r="AW67" s="66"/>
+      <c r="AX67" s="53"/>
+      <c r="AY67" s="66"/>
+      <c r="AZ67" s="66"/>
+      <c r="BA67" s="66"/>
       <c r="BB67" s="6"/>
       <c r="BC67" s="6"/>
       <c r="BD67" s="6"/>
       <c r="BE67" s="6"/>
       <c r="BF67" s="47"/>
     </row>
-    <row r="68" spans="2:58">
+    <row r="68" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B68" s="47"/>
       <c r="C68" s="3" t="s">
         <v>106</v>
@@ -6417,20 +6490,20 @@
       <c r="AR68" s="6"/>
       <c r="AS68" s="6"/>
       <c r="AT68" s="6"/>
-      <c r="AU68" s="30"/>
-      <c r="AV68" s="6"/>
-      <c r="AW68" s="6"/>
-      <c r="AX68" s="6"/>
-      <c r="AY68" s="6"/>
-      <c r="AZ68" s="6"/>
-      <c r="BA68" s="6"/>
+      <c r="AU68" s="66"/>
+      <c r="AV68" s="66"/>
+      <c r="AW68" s="66"/>
+      <c r="AX68" s="66"/>
+      <c r="AY68" s="53"/>
+      <c r="AZ68" s="66"/>
+      <c r="BA68" s="66"/>
       <c r="BB68" s="6"/>
       <c r="BC68" s="6"/>
       <c r="BD68" s="6"/>
       <c r="BE68" s="6"/>
       <c r="BF68" s="47"/>
     </row>
-    <row r="69" spans="2:58">
+    <row r="69" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B69" s="47"/>
       <c r="C69" s="3" t="s">
         <v>107</v>
@@ -6480,22 +6553,22 @@
       <c r="AP69" s="21"/>
       <c r="AQ69" s="47"/>
       <c r="AR69" s="6"/>
-      <c r="AS69" s="30"/>
-      <c r="AT69" s="6"/>
-      <c r="AU69" s="6"/>
-      <c r="AV69" s="6"/>
-      <c r="AW69" s="6"/>
-      <c r="AX69" s="6"/>
-      <c r="AY69" s="6"/>
-      <c r="AZ69" s="6"/>
-      <c r="BA69" s="6"/>
+      <c r="AS69" s="6"/>
+      <c r="AT69" s="66"/>
+      <c r="AU69" s="66"/>
+      <c r="AV69" s="66"/>
+      <c r="AW69" s="66"/>
+      <c r="AX69" s="66"/>
+      <c r="AY69" s="53"/>
+      <c r="AZ69" s="66"/>
+      <c r="BA69" s="66"/>
       <c r="BB69" s="6"/>
       <c r="BC69" s="6"/>
       <c r="BD69" s="6"/>
       <c r="BE69" s="6"/>
       <c r="BF69" s="47"/>
     </row>
-    <row r="70" spans="2:58">
+    <row r="70" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B70" s="47"/>
       <c r="C70" s="3" t="s">
         <v>108</v>
@@ -6545,22 +6618,22 @@
       <c r="AP70" s="21"/>
       <c r="AQ70" s="47"/>
       <c r="AR70" s="6"/>
-      <c r="AS70" s="30"/>
-      <c r="AT70" s="6"/>
-      <c r="AU70" s="6"/>
-      <c r="AV70" s="6"/>
-      <c r="AW70" s="6"/>
-      <c r="AX70" s="6"/>
-      <c r="AY70" s="6"/>
-      <c r="AZ70" s="6"/>
-      <c r="BA70" s="6"/>
+      <c r="AS70" s="6"/>
+      <c r="AT70" s="66"/>
+      <c r="AU70" s="66"/>
+      <c r="AV70" s="66"/>
+      <c r="AW70" s="66"/>
+      <c r="AX70" s="66"/>
+      <c r="AY70" s="53"/>
+      <c r="AZ70" s="66"/>
+      <c r="BA70" s="66"/>
       <c r="BB70" s="6"/>
       <c r="BC70" s="6"/>
       <c r="BD70" s="6"/>
       <c r="BE70" s="6"/>
       <c r="BF70" s="47"/>
     </row>
-    <row r="71" spans="2:58">
+    <row r="71" spans="2:58" x14ac:dyDescent="0.25">
       <c r="B71" s="47"/>
       <c r="C71" s="3" t="s">
         <v>109</v>
@@ -6610,22 +6683,22 @@
       <c r="AP71" s="21"/>
       <c r="AQ71" s="47"/>
       <c r="AR71" s="6"/>
-      <c r="AS71" s="30"/>
-      <c r="AT71" s="6"/>
-      <c r="AU71" s="6"/>
-      <c r="AV71" s="6"/>
-      <c r="AW71" s="6"/>
-      <c r="AX71" s="6"/>
-      <c r="AY71" s="6"/>
-      <c r="AZ71" s="6"/>
-      <c r="BA71" s="6"/>
+      <c r="AS71" s="6"/>
+      <c r="AT71" s="66"/>
+      <c r="AU71" s="66"/>
+      <c r="AV71" s="66"/>
+      <c r="AW71" s="66"/>
+      <c r="AX71" s="66"/>
+      <c r="AY71" s="53"/>
+      <c r="AZ71" s="66"/>
+      <c r="BA71" s="66"/>
       <c r="BB71" s="6"/>
       <c r="BC71" s="6"/>
       <c r="BD71" s="6"/>
       <c r="BE71" s="6"/>
       <c r="BF71" s="47"/>
     </row>
-    <row r="72" spans="2:58" ht="8" customHeight="1">
+    <row r="72" spans="2:58" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="48"/>
       <c r="C72" s="11"/>
       <c r="D72" s="12"/>
@@ -6686,18 +6759,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G31:AP31"/>
+    <mergeCell ref="G30:AP30"/>
+    <mergeCell ref="G44:AP44"/>
+    <mergeCell ref="G47:AP47"/>
+    <mergeCell ref="G64:AP64"/>
+    <mergeCell ref="G63:AP63"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="G11:AP11"/>
     <mergeCell ref="G24:AP24"/>
     <mergeCell ref="G25:AP25"/>
     <mergeCell ref="G13:AP13"/>
     <mergeCell ref="G14:AP14"/>
-    <mergeCell ref="G31:AP31"/>
-    <mergeCell ref="G30:AP30"/>
-    <mergeCell ref="G44:AP44"/>
-    <mergeCell ref="G47:AP47"/>
-    <mergeCell ref="G64:AP64"/>
-    <mergeCell ref="G63:AP63"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>